<commit_message>
Update median of clusters (normbysoul) no mundist.xlsx
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/median of clusters (normbysoul) no mundist.xlsx
+++ b/migforecasting/clustering/median of clusters (normbysoul) no mundist.xlsx
@@ -489,7 +489,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,6 +905,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C7">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -916,7 +928,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="E2:E7">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -928,7 +940,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E7">
+  <conditionalFormatting sqref="F2:F7">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -940,7 +952,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F7">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -952,7 +964,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -964,7 +976,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -976,7 +988,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -988,7 +1000,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="K2:K7">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -1000,7 +1012,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K7">
+  <conditionalFormatting sqref="L2:L7">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1012,7 +1024,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L7">
+  <conditionalFormatting sqref="M2:M7">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1024,7 +1036,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M7">
+  <conditionalFormatting sqref="N2:N7">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1036,7 +1048,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N7">
+  <conditionalFormatting sqref="O2:O7">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1048,7 +1060,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O7">
+  <conditionalFormatting sqref="P2:P7">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1060,7 +1072,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P7">
+  <conditionalFormatting sqref="Q2:Q7">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1072,7 +1084,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q7">
+  <conditionalFormatting sqref="R2:R7">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1084,7 +1096,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R7">
+  <conditionalFormatting sqref="B2:B7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>